<commit_message>
Commit 6 For Rewritten Code(Solved an Error)
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -181,7 +181,7 @@
     <t xml:space="preserve">D. Allows only specified users into Salesforce Org.</t>
   </si>
   <si>
-    <t xml:space="preserve"> What is the value of x after the code segment executes?&lt;code&gt;String x = 'A';Integer i = 10;if ( i &lt; 15 ) {i = 15;x = 'B';} else if ( i &lt; 20 ) {x = 'C';} else {x = 'D'; }&lt;/code&gt;</t>
+    <t xml:space="preserve"> What is the value of x after the code segment executes?&lt;code&gt;String x = 'A';Integer i = 10;if ( i &lt; 15 ) {i = 15;x = 'B';} else if ( i &lt; 20 ) {x = 'C';} else {x = 'D'; } &lt;/code&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">A. D </t>
@@ -917,8 +917,8 @@
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Commit 7 For Rewriiten Code(made small changes 2)
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -222,8 +222,8 @@
   </sheetPr>
   <dimension ref="A1:H194"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -285,7 +285,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0</v>
@@ -311,13 +311,13 @@
         <v>15</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="86.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -337,13 +337,13 @@
         <v>19</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="100.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -363,7 +363,7 @@
         <v>26</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>0</v>
@@ -389,7 +389,7 @@
         <v>29</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>0</v>

</xml_diff>